<commit_message>
Minor corrections and changes
</commit_message>
<xml_diff>
--- a/app/help/@about.xlsx
+++ b/app/help/@about.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="28035" windowHeight="14130"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="28035" windowHeight="14130" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Desc" sheetId="9" r:id="rId1"/>
@@ -1768,16 +1768,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="7" width="37.7109375" style="1" customWidth="1"/>
+    <col min="1" max="7" width="43.5703125" style="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -2334,7 +2334,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C55" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>